<commit_message>
2 obj results - Berlin
Signed-off-by: Ursidean <charlesnewlandprofessional@outlook.com>
</commit_message>
<xml_diff>
--- a/EU_output/Coarse parameter analysis 3obj.xlsx
+++ b/EU_output/Coarse parameter analysis 3obj.xlsx
@@ -5,7 +5,7 @@
   <workbookPr filterPrivacy="1"/>
   <xr:revisionPtr revIDLastSave="200" documentId="C09621C0CEF46EDEE85F53CAB52B596D5051CF5D" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{B69C7B45-9D77-45B1-89E6-9B7FCFAED338}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Berlin" sheetId="1" r:id="rId1"/>
@@ -4418,7 +4418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
@@ -12911,7 +12911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E8FAE7-2671-4E29-9981-4FFC9A9801D9}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>